<commit_message>
support for yaml doc
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="109">
   <si>
     <t>Q123456</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -38,10 +38,6 @@
   </si>
   <si>
     <t>用户昵称</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>接口地址</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -198,22 +194,6 @@
   </si>
   <si>
     <r>
-      <t>EOMS</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="微软雅黑"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>接口文档</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
       <rPr>
         <b/>
         <sz val="12"/>
@@ -235,14 +215,6 @@
       </rPr>
       <t>测试数据</t>
     </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>请求Headers</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>响应Headers</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -531,6 +503,50 @@
   </si>
   <si>
     <t>账号登录</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Example </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>接口文档</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Response Headers</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Request Headers</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>接口</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>方法</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>权限</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>接口</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>接口</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -849,7 +865,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -981,22 +997,28 @@
     <xf numFmtId="0" fontId="11" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1318,12 +1340,12 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="18.125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="19.625" style="1" customWidth="1"/>
     <col min="2" max="2" width="31.625" style="1" customWidth="1"/>
     <col min="3" max="3" width="42.75" style="1" customWidth="1"/>
     <col min="4" max="16384" width="9" style="1"/>
@@ -1331,35 +1353,35 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>42</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B2" s="3"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>36</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C4" s="42" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.4">
@@ -1367,28 +1389,28 @@
       <c r="B5" s="3"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A7" s="23" t="s">
-        <v>45</v>
+      <c r="A7" s="46" t="s">
+        <v>103</v>
       </c>
       <c r="B7" s="34" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A8" s="31"/>
       <c r="B8" s="31" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C8" s="32" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A9" s="23" t="s">
-        <v>46</v>
+      <c r="A9" s="46" t="s">
+        <v>102</v>
       </c>
       <c r="B9" s="34"/>
       <c r="C9" s="20"/>
@@ -1396,10 +1418,10 @@
     <row r="10" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A10" s="31"/>
       <c r="B10" s="31" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C10" s="32" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1419,7 +1441,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="6" topLeftCell="G1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B2" sqref="B2:D2"/>
+      <selection pane="topRight" activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
@@ -1434,13 +1456,13 @@
   <sheetData>
     <row r="1" spans="1:9" s="9" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B1" s="47" t="s">
-        <v>54</v>
-      </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
+        <v>43</v>
+      </c>
+      <c r="B1" s="49" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
       <c r="E1" s="29"/>
       <c r="F1" s="8"/>
       <c r="G1" s="18"/>
@@ -1449,13 +1471,13 @@
     </row>
     <row r="2" spans="1:9" s="9" customFormat="1" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" s="51" t="s">
-        <v>104</v>
-      </c>
-      <c r="C2" s="50"/>
-      <c r="D2" s="52"/>
+        <v>100</v>
+      </c>
+      <c r="C2" s="52"/>
+      <c r="D2" s="53"/>
       <c r="E2" s="29"/>
       <c r="F2" s="8"/>
       <c r="G2" s="18"/>
@@ -1463,14 +1485,14 @@
       <c r="I2" s="18"/>
     </row>
     <row r="3" spans="1:9" s="9" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="49" t="s">
-        <v>52</v>
-      </c>
-      <c r="C3" s="50"/>
-      <c r="D3" s="52"/>
+      <c r="A3" s="47" t="s">
+        <v>107</v>
+      </c>
+      <c r="B3" s="54" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="52"/>
+      <c r="D3" s="53"/>
       <c r="E3" s="10"/>
       <c r="F3" s="8"/>
       <c r="G3" s="15"/>
@@ -1478,28 +1500,28 @@
       <c r="I3" s="15"/>
     </row>
     <row r="4" spans="1:9" s="9" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="49" t="s">
-        <v>50</v>
-      </c>
-      <c r="C4" s="50"/>
-      <c r="D4" s="52"/>
+      <c r="A4" s="47" t="s">
+        <v>105</v>
+      </c>
+      <c r="B4" s="54" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="52"/>
+      <c r="D4" s="53"/>
       <c r="E4" s="29"/>
       <c r="G4" s="15"/>
       <c r="H4" s="15"/>
       <c r="I4" s="15"/>
     </row>
     <row r="5" spans="1:9" s="9" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="53" t="s">
-        <v>51</v>
-      </c>
-      <c r="C5" s="54"/>
-      <c r="D5" s="55"/>
+      <c r="A5" s="48" t="s">
+        <v>106</v>
+      </c>
+      <c r="B5" s="55" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="56"/>
+      <c r="D5" s="57"/>
       <c r="E5" s="30"/>
       <c r="G5" s="15"/>
       <c r="H5" s="15"/>
@@ -1507,46 +1529,46 @@
     </row>
     <row r="6" spans="1:9" s="7" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A6" s="23" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="D6" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="23" t="s">
+      <c r="E6" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="23" t="s">
+      <c r="F6" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="23" t="s">
-        <v>28</v>
-      </c>
       <c r="G6" s="33" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:9" s="14" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A7" s="27"/>
       <c r="B7" s="20" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D7" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="12" t="s">
         <v>30</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>31</v>
       </c>
       <c r="F7" s="11"/>
       <c r="G7" s="13" t="s">
@@ -1556,7 +1578,7 @@
         <v>3</v>
       </c>
       <c r="I7" s="14" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8" spans="1:9" s="17" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.2">
@@ -1565,28 +1587,28 @@
         <v>2</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D8" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="12" t="s">
         <v>30</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>31</v>
       </c>
       <c r="F8" s="11"/>
       <c r="G8" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H8" s="14" t="s">
         <v>0</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="7" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A9" s="23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B9" s="23"/>
       <c r="C9" s="23"/>
@@ -1606,49 +1628,49 @@
     <row r="10" spans="1:9" s="16" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A10" s="27"/>
       <c r="B10" s="22" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C10" s="25" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="H10" s="14" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I10" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:9" s="14" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A11" s="27"/>
       <c r="B11" s="20" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C11" s="26" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F11" s="11" t="s">
         <v>5</v>
       </c>
       <c r="G11" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H11" s="14" t="s">
         <v>4</v>
@@ -1656,7 +1678,7 @@
     </row>
     <row r="12" spans="1:9" s="43" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A12" s="46" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B12" s="23"/>
       <c r="C12" s="23"/>
@@ -1667,12 +1689,12 @@
         <v>0.5</v>
       </c>
       <c r="I12" s="43">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:9" s="6" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A13" s="46" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13" s="23"/>
       <c r="C13" s="23"/>
@@ -1680,25 +1702,25 @@
       <c r="E13" s="23"/>
       <c r="F13" s="23"/>
       <c r="G13" s="45" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="H13" s="14" t="s">
         <v>4</v>
       </c>
       <c r="I13" s="14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="15" spans="1:9" s="9" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B15" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="C15" s="48"/>
-      <c r="D15" s="48"/>
+        <v>44</v>
+      </c>
+      <c r="B15" s="49" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" s="50"/>
+      <c r="D15" s="50"/>
       <c r="E15" s="29"/>
       <c r="F15" s="8"/>
       <c r="G15" s="18"/>
@@ -1707,13 +1729,13 @@
     </row>
     <row r="16" spans="1:9" s="9" customFormat="1" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16" s="51" t="s">
-        <v>103</v>
-      </c>
-      <c r="C16" s="50"/>
-      <c r="D16" s="50"/>
+        <v>99</v>
+      </c>
+      <c r="C16" s="52"/>
+      <c r="D16" s="52"/>
       <c r="E16" s="29"/>
       <c r="F16" s="8"/>
       <c r="G16" s="18"/>
@@ -1721,14 +1743,14 @@
       <c r="I16" s="18"/>
     </row>
     <row r="17" spans="1:9" s="9" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B17" s="49" t="s">
-        <v>85</v>
-      </c>
-      <c r="C17" s="50"/>
-      <c r="D17" s="50"/>
+      <c r="A17" s="47" t="s">
+        <v>108</v>
+      </c>
+      <c r="B17" s="54" t="s">
+        <v>81</v>
+      </c>
+      <c r="C17" s="52"/>
+      <c r="D17" s="52"/>
       <c r="E17" s="29"/>
       <c r="F17" s="8"/>
       <c r="G17" s="15"/>
@@ -1737,13 +1759,13 @@
     </row>
     <row r="18" spans="1:9" s="9" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18" s="49" t="s">
-        <v>60</v>
-      </c>
-      <c r="C18" s="50"/>
-      <c r="D18" s="50"/>
+        <v>7</v>
+      </c>
+      <c r="B18" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" s="52"/>
+      <c r="D18" s="52"/>
       <c r="E18" s="29"/>
       <c r="G18" s="15"/>
       <c r="H18" s="15"/>
@@ -1751,13 +1773,13 @@
     </row>
     <row r="19" spans="1:9" s="9" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A19" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="B19" s="56" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19" s="57"/>
-      <c r="D19" s="57"/>
+        <v>6</v>
+      </c>
+      <c r="B19" s="58" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="59"/>
+      <c r="D19" s="59"/>
       <c r="E19" s="30"/>
       <c r="G19" s="15"/>
       <c r="H19" s="15"/>
@@ -1765,63 +1787,63 @@
     </row>
     <row r="20" spans="1:9" s="7" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A20" s="23" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B20" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="23" t="s">
+      <c r="D20" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="23" t="s">
+      <c r="E20" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="E20" s="23" t="s">
+      <c r="F20" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="F20" s="23" t="s">
-        <v>28</v>
-      </c>
       <c r="G20" s="28" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H20" s="28" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:9" s="37" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A21" s="27" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C21" s="11"/>
       <c r="D21" s="12"/>
       <c r="E21" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F21" s="11"/>
       <c r="G21" s="38" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="H21" s="38"/>
     </row>
     <row r="22" spans="1:9" s="14" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A22" s="27" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F22" s="11"/>
       <c r="G22" s="13">
@@ -1834,43 +1856,43 @@
     <row r="23" spans="1:9" s="35" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A23" s="27"/>
       <c r="B23" s="20" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F23" s="11"/>
       <c r="G23" s="36" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="H23" s="38" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:9" s="7" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A24" s="23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B24" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="C24" s="23" t="s">
+      <c r="D24" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="D24" s="23" t="s">
+      <c r="E24" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="E24" s="23" t="s">
+      <c r="F24" s="23" t="s">
         <v>27</v>
-      </c>
-      <c r="F24" s="23" t="s">
-        <v>28</v>
       </c>
       <c r="G24" s="28">
         <v>200</v>
@@ -1882,31 +1904,31 @@
     <row r="25" spans="1:9" s="16" customFormat="1" ht="72.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A25" s="27"/>
       <c r="B25" s="22" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C25" s="25" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F25" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G25" s="13" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="H25" s="40" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="I25" s="14"/>
     </row>
     <row r="26" spans="1:9" s="6" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A26" s="23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B26" s="23"/>
       <c r="C26" s="23"/>
@@ -1914,7 +1936,7 @@
       <c r="E26" s="23"/>
       <c r="F26" s="23"/>
       <c r="G26" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H26" s="14"/>
       <c r="I26" s="14"/>
@@ -1922,13 +1944,13 @@
     <row r="27" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="28" spans="1:9" s="9" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B28" s="47" t="s">
-        <v>67</v>
-      </c>
-      <c r="C28" s="48"/>
-      <c r="D28" s="48"/>
+        <v>45</v>
+      </c>
+      <c r="B28" s="49" t="s">
+        <v>63</v>
+      </c>
+      <c r="C28" s="50"/>
+      <c r="D28" s="50"/>
       <c r="E28" s="29"/>
       <c r="F28" s="8"/>
       <c r="G28" s="18"/>
@@ -1937,13 +1959,13 @@
     </row>
     <row r="29" spans="1:9" s="9" customFormat="1" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B29" s="51" t="s">
-        <v>102</v>
-      </c>
-      <c r="C29" s="50"/>
-      <c r="D29" s="50"/>
+        <v>98</v>
+      </c>
+      <c r="C29" s="52"/>
+      <c r="D29" s="52"/>
       <c r="E29" s="29"/>
       <c r="F29" s="8"/>
       <c r="G29" s="18"/>
@@ -1951,14 +1973,14 @@
       <c r="I29" s="18"/>
     </row>
     <row r="30" spans="1:9" s="9" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B30" s="49" t="s">
-        <v>89</v>
-      </c>
-      <c r="C30" s="50"/>
-      <c r="D30" s="50"/>
+      <c r="A30" s="47" t="s">
+        <v>104</v>
+      </c>
+      <c r="B30" s="54" t="s">
+        <v>85</v>
+      </c>
+      <c r="C30" s="52"/>
+      <c r="D30" s="52"/>
       <c r="E30" s="29"/>
       <c r="F30" s="8"/>
       <c r="G30" s="15"/>
@@ -1967,13 +1989,13 @@
     </row>
     <row r="31" spans="1:9" s="9" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B31" s="49" t="s">
-        <v>59</v>
-      </c>
-      <c r="C31" s="50"/>
-      <c r="D31" s="50"/>
+        <v>7</v>
+      </c>
+      <c r="B31" s="54" t="s">
+        <v>55</v>
+      </c>
+      <c r="C31" s="52"/>
+      <c r="D31" s="52"/>
       <c r="E31" s="29"/>
       <c r="G31" s="15"/>
       <c r="H31" s="15"/>
@@ -1981,13 +2003,13 @@
     </row>
     <row r="32" spans="1:9" s="9" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A32" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="B32" s="56" t="s">
-        <v>18</v>
-      </c>
-      <c r="C32" s="57"/>
-      <c r="D32" s="57"/>
+        <v>6</v>
+      </c>
+      <c r="B32" s="58" t="s">
+        <v>17</v>
+      </c>
+      <c r="C32" s="59"/>
+      <c r="D32" s="59"/>
       <c r="E32" s="30"/>
       <c r="G32" s="15"/>
       <c r="H32" s="15"/>
@@ -1995,76 +2017,76 @@
     </row>
     <row r="33" spans="1:9" s="7" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A33" s="23" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B33" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="C33" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="C33" s="23" t="s">
+      <c r="D33" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="D33" s="23" t="s">
+      <c r="E33" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="E33" s="23" t="s">
+      <c r="F33" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="F33" s="23" t="s">
-        <v>28</v>
-      </c>
       <c r="G33" s="28" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H33" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I33" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="34" spans="1:9" s="14" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A34" s="27"/>
       <c r="B34" s="20" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D34" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="E34" s="12" t="s">
         <v>30</v>
-      </c>
-      <c r="E34" s="12" t="s">
-        <v>31</v>
       </c>
       <c r="F34" s="11"/>
       <c r="G34" s="41" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="H34" s="41" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="I34" s="41" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="35" spans="1:9" s="7" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A35" s="23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B35" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="C35" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="C35" s="23" t="s">
+      <c r="D35" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="D35" s="23" t="s">
+      <c r="E35" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="E35" s="23" t="s">
+      <c r="F35" s="23" t="s">
         <v>27</v>
-      </c>
-      <c r="F35" s="23" t="s">
-        <v>28</v>
       </c>
       <c r="G35" s="28">
         <v>200</v>
@@ -2079,33 +2101,33 @@
     <row r="36" spans="1:9" s="16" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A36" s="27"/>
       <c r="B36" s="22" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C36" s="25" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D36" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E36" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F36" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G36" s="13" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="H36" s="38" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="I36" s="38" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="37" spans="1:9" s="6" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A37" s="23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B37" s="23"/>
       <c r="C37" s="23"/>
@@ -2113,13 +2135,13 @@
       <c r="E37" s="23"/>
       <c r="F37" s="23"/>
       <c r="G37" s="13" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="H37" s="14" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="I37" s="39" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update the Readme for Apistar versin
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7770" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7770"/>
   </bookViews>
   <sheets>
     <sheet name="INDEX" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="115">
   <si>
     <t>Q123456</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -495,6 +495,68 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>Response Headers</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Request Headers</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>接口</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>方法</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>权限</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>接口</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>接口</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>*</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+    "code": "0",
+    "message": "success"
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+    "code": "0",
+    "message": "success"
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>guess</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>填写任意密码都可以通过</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>*</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>guess</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">Example </t>
     </r>
@@ -502,8 +564,8 @@
       <rPr>
         <sz val="14"/>
         <color theme="1"/>
-        <rFont val="微软雅黑"/>
-        <family val="2"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>接口文档</t>
@@ -511,65 +573,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Response Headers</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Request Headers</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>接口</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>方法</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>权限</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>接口</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>接口</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>*</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{
-    "code": "0",
-    "message": "success"
-}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{
-    "code": "0",
-    "message": "success"
-}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>guess</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>填写任意密码都可以通过</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>*</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>guess</t>
+    <t>Example</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -577,7 +581,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -603,13 +607,6 @@
       <color theme="0"/>
       <name val="Open Sans"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="微软雅黑"/>
-      <family val="2"/>
-      <charset val="134"/>
     </font>
     <font>
       <b/>
@@ -896,176 +893,176 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="22" fontId="8" fillId="2" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="22" fontId="9" fillId="2" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1371,8 +1368,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.4"/>
@@ -1388,14 +1385,16 @@
         <v>33</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>99</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="3"/>
+      <c r="B2" s="3" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
@@ -1422,7 +1421,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7" s="46" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B7" s="34" t="s">
         <v>41</v>
@@ -1442,7 +1441,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A9" s="46" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B9" s="34"/>
       <c r="C9" s="20"/>
@@ -1471,7 +1470,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="6" topLeftCell="G1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="D59" sqref="D59"/>
     </sheetView>
@@ -1493,11 +1492,11 @@
       <c r="A1" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="52" t="s">
+      <c r="B1" s="56" t="s">
         <v>50</v>
       </c>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
       <c r="E1" s="29"/>
       <c r="F1" s="8"/>
       <c r="G1" s="18"/>
@@ -1508,11 +1507,11 @@
       <c r="A2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="58" t="s">
         <v>98</v>
       </c>
-      <c r="C2" s="55"/>
-      <c r="D2" s="56"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="59"/>
       <c r="E2" s="29"/>
       <c r="F2" s="8"/>
       <c r="G2" s="18"/>
@@ -1521,13 +1520,13 @@
     </row>
     <row r="3" spans="1:10" s="9" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A3" s="47" t="s">
-        <v>105</v>
-      </c>
-      <c r="B3" s="57" t="s">
+        <v>104</v>
+      </c>
+      <c r="B3" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="C3" s="55"/>
-      <c r="D3" s="56"/>
+      <c r="C3" s="53"/>
+      <c r="D3" s="59"/>
       <c r="E3" s="10"/>
       <c r="F3" s="8"/>
       <c r="G3" s="15"/>
@@ -1536,13 +1535,13 @@
     </row>
     <row r="4" spans="1:10" s="9" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A4" s="47" t="s">
-        <v>103</v>
-      </c>
-      <c r="B4" s="57" t="s">
+        <v>102</v>
+      </c>
+      <c r="B4" s="52" t="s">
         <v>46</v>
       </c>
-      <c r="C4" s="55"/>
-      <c r="D4" s="56"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="59"/>
       <c r="E4" s="29"/>
       <c r="G4" s="15"/>
       <c r="H4" s="15"/>
@@ -1550,13 +1549,13 @@
     </row>
     <row r="5" spans="1:10" s="9" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A5" s="48" t="s">
-        <v>104</v>
-      </c>
-      <c r="B5" s="58" t="s">
+        <v>103</v>
+      </c>
+      <c r="B5" s="60" t="s">
         <v>47</v>
       </c>
-      <c r="C5" s="59"/>
-      <c r="D5" s="60"/>
+      <c r="C5" s="61"/>
+      <c r="D5" s="62"/>
       <c r="E5" s="30"/>
       <c r="G5" s="15"/>
       <c r="H5" s="15"/>
@@ -1619,7 +1618,7 @@
         <v>93</v>
       </c>
       <c r="J7" s="14" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" spans="1:10" s="17" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.2">
@@ -1644,10 +1643,10 @@
         <v>0</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J8" s="17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:10" s="7" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.2">
@@ -1690,7 +1689,7 @@
         <v>21</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H10" s="14" t="s">
         <v>69</v>
@@ -1699,7 +1698,7 @@
         <v>32</v>
       </c>
       <c r="J10" s="16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="11" spans="1:10" s="14" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.2">
@@ -1726,7 +1725,7 @@
         <v>4</v>
       </c>
       <c r="J11" s="49" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="12" spans="1:10" s="43" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.2">
@@ -1764,7 +1763,7 @@
         <v>10</v>
       </c>
       <c r="J13" s="50" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.2"/>
@@ -1772,11 +1771,11 @@
       <c r="A15" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B15" s="52" t="s">
+      <c r="B15" s="56" t="s">
         <v>49</v>
       </c>
-      <c r="C15" s="53"/>
-      <c r="D15" s="53"/>
+      <c r="C15" s="57"/>
+      <c r="D15" s="57"/>
       <c r="E15" s="29"/>
       <c r="F15" s="8"/>
       <c r="G15" s="18"/>
@@ -1787,11 +1786,11 @@
       <c r="A16" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="54" t="s">
+      <c r="B16" s="58" t="s">
         <v>97</v>
       </c>
-      <c r="C16" s="55"/>
-      <c r="D16" s="55"/>
+      <c r="C16" s="53"/>
+      <c r="D16" s="53"/>
       <c r="E16" s="29"/>
       <c r="F16" s="8"/>
       <c r="G16" s="18"/>
@@ -1800,13 +1799,13 @@
     </row>
     <row r="17" spans="1:9" s="9" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A17" s="47" t="s">
-        <v>106</v>
-      </c>
-      <c r="B17" s="57" t="s">
+        <v>105</v>
+      </c>
+      <c r="B17" s="52" t="s">
         <v>80</v>
       </c>
-      <c r="C17" s="55"/>
-      <c r="D17" s="55"/>
+      <c r="C17" s="53"/>
+      <c r="D17" s="53"/>
       <c r="E17" s="29"/>
       <c r="F17" s="8"/>
       <c r="G17" s="15"/>
@@ -1817,11 +1816,11 @@
       <c r="A18" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B18" s="57" t="s">
+      <c r="B18" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="C18" s="55"/>
-      <c r="D18" s="55"/>
+      <c r="C18" s="53"/>
+      <c r="D18" s="53"/>
       <c r="E18" s="29"/>
       <c r="G18" s="15"/>
       <c r="H18" s="15"/>
@@ -1831,11 +1830,11 @@
       <c r="A19" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="61" t="s">
+      <c r="B19" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="62"/>
-      <c r="D19" s="62"/>
+      <c r="C19" s="55"/>
+      <c r="D19" s="55"/>
       <c r="E19" s="30"/>
       <c r="G19" s="15"/>
       <c r="H19" s="15"/>
@@ -2002,11 +2001,11 @@
       <c r="A28" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B28" s="52" t="s">
+      <c r="B28" s="56" t="s">
         <v>63</v>
       </c>
-      <c r="C28" s="53"/>
-      <c r="D28" s="53"/>
+      <c r="C28" s="57"/>
+      <c r="D28" s="57"/>
       <c r="E28" s="29"/>
       <c r="F28" s="8"/>
       <c r="G28" s="18"/>
@@ -2017,11 +2016,11 @@
       <c r="A29" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B29" s="54" t="s">
+      <c r="B29" s="58" t="s">
         <v>96</v>
       </c>
-      <c r="C29" s="55"/>
-      <c r="D29" s="55"/>
+      <c r="C29" s="53"/>
+      <c r="D29" s="53"/>
       <c r="E29" s="29"/>
       <c r="F29" s="8"/>
       <c r="G29" s="18"/>
@@ -2030,13 +2029,13 @@
     </row>
     <row r="30" spans="1:9" s="9" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A30" s="47" t="s">
-        <v>102</v>
-      </c>
-      <c r="B30" s="57" t="s">
+        <v>101</v>
+      </c>
+      <c r="B30" s="52" t="s">
         <v>84</v>
       </c>
-      <c r="C30" s="55"/>
-      <c r="D30" s="55"/>
+      <c r="C30" s="53"/>
+      <c r="D30" s="53"/>
       <c r="E30" s="29"/>
       <c r="F30" s="8"/>
       <c r="G30" s="15"/>
@@ -2047,11 +2046,11 @@
       <c r="A31" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B31" s="57" t="s">
+      <c r="B31" s="52" t="s">
         <v>55</v>
       </c>
-      <c r="C31" s="55"/>
-      <c r="D31" s="55"/>
+      <c r="C31" s="53"/>
+      <c r="D31" s="53"/>
       <c r="E31" s="29"/>
       <c r="G31" s="15"/>
       <c r="H31" s="15"/>
@@ -2061,11 +2060,11 @@
       <c r="A32" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B32" s="61" t="s">
+      <c r="B32" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="C32" s="62"/>
-      <c r="D32" s="62"/>
+      <c r="C32" s="55"/>
+      <c r="D32" s="55"/>
       <c r="E32" s="30"/>
       <c r="G32" s="15"/>
       <c r="H32" s="15"/>
@@ -2202,6 +2201,13 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B5:D5"/>
     <mergeCell ref="B31:D31"/>
     <mergeCell ref="B32:D32"/>
     <mergeCell ref="B17:D17"/>
@@ -2210,13 +2216,6 @@
     <mergeCell ref="B28:D28"/>
     <mergeCell ref="B29:D29"/>
     <mergeCell ref="B30:D30"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B5:D5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="4">

</xml_diff>